<commit_message>
updated business logic for the july law changes
</commit_message>
<xml_diff>
--- a/DATA.xlsx
+++ b/DATA.xlsx
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="82">
-  <si>
-    <t>20-215-6347</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="80">
   <si>
     <t>Telefon</t>
   </si>
@@ -235,9 +232,6 @@
   </si>
   <si>
     <t>20-954-8725</t>
-  </si>
-  <si>
-    <t>20-964-5666</t>
   </si>
   <si>
     <t>30-224-7205</t>
@@ -589,7 +583,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D312"/>
+  <dimension ref="A1:D308"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -597,13 +591,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1">
-        <v>28.49</v>
+        <v>3700</v>
       </c>
       <c r="D1" t="b">
         <v>0</v>
@@ -611,13 +605,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>3964</v>
+        <v>0.01</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -625,13 +619,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -639,13 +633,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
@@ -653,13 +647,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5">
-        <v>2718.08</v>
+        <v>1387</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
@@ -667,10 +661,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <v>2191.36</v>
@@ -681,10 +675,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7">
         <v>4980</v>
@@ -695,10 +689,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -709,10 +703,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9">
         <v>1905</v>
@@ -723,10 +717,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <v>1261.24</v>
@@ -737,10 +731,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -751,10 +745,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -765,13 +759,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <v>2038.35</v>
+        <v>1924.05</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
@@ -779,10 +773,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <v>1261.24</v>
@@ -793,10 +787,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -807,10 +801,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -821,13 +815,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D17" t="b">
         <v>0</v>
@@ -835,10 +829,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18">
         <v>570.46</v>
@@ -849,10 +843,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -863,10 +857,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -877,13 +871,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21">
-        <v>2623.66</v>
+        <v>2454.66</v>
       </c>
       <c r="D21" t="b">
         <v>0</v>
@@ -891,10 +885,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C22">
         <v>1261.24</v>
@@ -905,10 +899,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -919,10 +913,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -933,13 +927,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25">
-        <v>1924.04</v>
+        <v>1905</v>
       </c>
       <c r="D25" t="b">
         <v>0</v>
@@ -947,10 +941,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26">
         <v>1261.24</v>
@@ -961,10 +955,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -975,10 +969,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -989,13 +983,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29">
-        <v>1904.99</v>
+        <v>1905</v>
       </c>
       <c r="D29" t="b">
         <v>0</v>
@@ -1003,10 +997,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C30">
         <v>1261.24</v>
@@ -1017,10 +1011,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -1031,10 +1025,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B32" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -1045,10 +1039,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B33" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C33">
         <v>1905</v>
@@ -1059,10 +1053,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B34" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C34">
         <v>1261.24</v>
@@ -1073,10 +1067,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -1087,10 +1081,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -1101,13 +1095,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B37" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C37">
-        <v>2031.56</v>
+        <v>2057.4</v>
       </c>
       <c r="D37" t="b">
         <v>0</v>
@@ -1115,10 +1109,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B38" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C38">
         <v>2191.36</v>
@@ -1129,10 +1123,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B39" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1143,10 +1137,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B40" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1157,10 +1151,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B41" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C41">
         <v>1905</v>
@@ -1171,10 +1165,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C42">
         <v>1261.24</v>
@@ -1185,10 +1179,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B43" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -1199,10 +1193,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -1213,13 +1207,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B45" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C45">
-        <v>1924.05</v>
+        <v>1905</v>
       </c>
       <c r="D45" t="b">
         <v>0</v>
@@ -1227,10 +1221,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B46" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C46">
         <v>2191.36</v>
@@ -1241,10 +1235,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B47" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -1255,10 +1249,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B48" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -1269,13 +1263,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B49" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C49">
-        <v>1924.05</v>
+        <v>1943.1</v>
       </c>
       <c r="D49" t="b">
         <v>0</v>
@@ -1283,10 +1277,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B50" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C50">
         <v>1261.24</v>
@@ -1297,10 +1291,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B51" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -1311,10 +1305,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B52" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -1325,13 +1319,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B53" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C53">
-        <v>1904.99</v>
+        <v>1905.01</v>
       </c>
       <c r="D53" t="b">
         <v>0</v>
@@ -1339,10 +1333,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B54" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C54">
         <v>1261.24</v>
@@ -1353,13 +1347,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B55" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>3700</v>
       </c>
       <c r="D55" t="b">
         <v>0</v>
@@ -1367,10 +1361,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B56" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -1381,13 +1375,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B57" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C57">
-        <v>1904.98</v>
+        <v>1905</v>
       </c>
       <c r="D57" t="b">
         <v>0</v>
@@ -1395,10 +1389,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -1409,10 +1403,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B59" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -1423,10 +1417,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B60" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -1437,13 +1431,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B61" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C61">
-        <v>2305.04</v>
+        <v>2095.5</v>
       </c>
       <c r="D61" t="b">
         <v>0</v>
@@ -1451,10 +1445,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B62" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C62">
         <v>2191.36</v>
@@ -1465,10 +1459,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B63" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -1479,10 +1473,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B64" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -1493,10 +1487,10 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B65" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C65">
         <v>1905</v>
@@ -1507,10 +1501,10 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B66" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C66">
         <v>1261.24</v>
@@ -1521,10 +1515,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B67" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -1535,10 +1529,10 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B68" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -1549,13 +1543,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B69" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C69">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D69" t="b">
         <v>0</v>
@@ -1563,10 +1557,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B70" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C70">
         <v>570.46</v>
@@ -1577,10 +1571,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B71" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -1591,10 +1585,10 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B72" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -1605,13 +1599,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B73" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C73">
-        <v>28.49</v>
+        <v>0.01</v>
       </c>
       <c r="D73" t="b">
         <v>0</v>
@@ -1619,10 +1613,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B74" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C74">
         <v>570.46</v>
@@ -1633,10 +1627,10 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B75" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C75">
         <v>0</v>
@@ -1647,10 +1641,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B76" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C76">
         <v>0</v>
@@ -1661,13 +1655,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B77" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C77">
-        <v>2895.58</v>
+        <v>1905</v>
       </c>
       <c r="D77" t="b">
         <v>0</v>
@@ -1675,10 +1669,10 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B78" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C78">
         <v>2191.36</v>
@@ -1689,10 +1683,10 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B79" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C79">
         <v>0</v>
@@ -1703,10 +1697,10 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B80" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -1717,13 +1711,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B81" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D81" t="b">
         <v>0</v>
@@ -1731,10 +1725,10 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B82" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C82">
         <v>570.46</v>
@@ -1745,10 +1739,10 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B83" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -1759,10 +1753,10 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B84" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -1773,13 +1767,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B85" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C85">
-        <v>1924.04</v>
+        <v>1905</v>
       </c>
       <c r="D85" t="b">
         <v>0</v>
@@ -1787,10 +1781,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B86" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C86">
         <v>2191.36</v>
@@ -1801,10 +1795,10 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B87" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -1815,10 +1809,10 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B88" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -1829,13 +1823,13 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B89" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C89">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D89" t="b">
         <v>0</v>
@@ -1843,10 +1837,10 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B90" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C90">
         <v>570.46</v>
@@ -1857,10 +1851,10 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B91" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -1871,10 +1865,10 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B92" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C92">
         <v>0</v>
@@ -1885,13 +1879,13 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B93" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C93">
-        <v>1943.09</v>
+        <v>2187.96</v>
       </c>
       <c r="D93" t="b">
         <v>0</v>
@@ -1899,10 +1893,10 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B94" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C94">
         <v>1261.24</v>
@@ -1913,10 +1907,10 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B95" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C95">
         <v>0</v>
@@ -1927,10 +1921,10 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B96" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C96">
         <v>0</v>
@@ -1941,10 +1935,10 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B97" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C97">
         <v>1905</v>
@@ -1955,10 +1949,10 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B98" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C98">
         <v>1261.24</v>
@@ -1969,10 +1963,10 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B99" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C99">
         <v>0</v>
@@ -1983,10 +1977,10 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B100" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C100">
         <v>0</v>
@@ -1997,13 +1991,13 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B101" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C101">
-        <v>1943.1</v>
+        <v>1905</v>
       </c>
       <c r="D101" t="b">
         <v>0</v>
@@ -2011,10 +2005,10 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B102" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C102">
         <v>1261.24</v>
@@ -2025,10 +2019,10 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B103" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C103">
         <v>0</v>
@@ -2039,10 +2033,10 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B104" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C104">
         <v>0</v>
@@ -2053,10 +2047,10 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B105" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C105">
         <v>1905</v>
@@ -2067,10 +2061,10 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B106" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C106">
         <v>1261.24</v>
@@ -2081,10 +2075,10 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B107" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C107">
         <v>0</v>
@@ -2095,10 +2089,10 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B108" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C108">
         <v>0</v>
@@ -2109,13 +2103,13 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B109" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C109">
-        <v>2955.73</v>
+        <v>2903.83</v>
       </c>
       <c r="D109" t="b">
         <v>0</v>
@@ -2123,10 +2117,10 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B110" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C110">
         <v>2191.36</v>
@@ -2137,10 +2131,10 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B111" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C111">
         <v>0</v>
@@ -2151,10 +2145,10 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B112" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -2165,13 +2159,13 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B113" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C113">
-        <v>3738.71</v>
+        <v>4599.2700000000004</v>
       </c>
       <c r="D113" t="b">
         <v>0</v>
@@ -2179,10 +2173,10 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B114" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C114">
         <v>1707.7</v>
@@ -2193,10 +2187,10 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B115" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -2207,13 +2201,13 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B116" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C116">
-        <v>210</v>
+        <v>753</v>
       </c>
       <c r="D116" t="b">
         <v>0</v>
@@ -2221,10 +2215,10 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B117" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C117">
         <v>1905</v>
@@ -2235,10 +2229,10 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B118" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C118">
         <v>1707.7</v>
@@ -2249,10 +2243,10 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B119" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C119">
         <v>0</v>
@@ -2263,10 +2257,10 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B120" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C120">
         <v>0</v>
@@ -2277,13 +2271,13 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B121" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C121">
-        <v>1924.02</v>
+        <v>1962.15</v>
       </c>
       <c r="D121" t="b">
         <v>0</v>
@@ -2291,10 +2285,10 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B122" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C122">
         <v>1261.24</v>
@@ -2305,10 +2299,10 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B123" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C123">
         <v>0</v>
@@ -2319,10 +2313,10 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B124" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C124">
         <v>0</v>
@@ -2333,10 +2327,10 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B125" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C125">
         <v>1905</v>
@@ -2347,10 +2341,10 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B126" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C126">
         <v>1261.24</v>
@@ -2361,10 +2355,10 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B127" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C127">
         <v>0</v>
@@ -2375,10 +2369,10 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B128" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C128">
         <v>0</v>
@@ -2389,10 +2383,10 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B129" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C129">
         <v>1905</v>
@@ -2403,10 +2397,10 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B130" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C130">
         <v>1261.24</v>
@@ -2417,10 +2411,10 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B131" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C131">
         <v>0</v>
@@ -2431,10 +2425,10 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B132" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C132">
         <v>0</v>
@@ -2445,13 +2439,13 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B133" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C133">
-        <v>2038.35</v>
+        <v>1905</v>
       </c>
       <c r="D133" t="b">
         <v>0</v>
@@ -2459,10 +2453,10 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B134" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C134">
         <v>1261.24</v>
@@ -2473,10 +2467,10 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B135" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -2487,10 +2481,10 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B136" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C136">
         <v>0</v>
@@ -2501,13 +2495,13 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B137" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C137">
-        <v>2019.28</v>
+        <v>2019.3</v>
       </c>
       <c r="D137" t="b">
         <v>0</v>
@@ -2515,10 +2509,10 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B138" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C138">
         <v>1261.24</v>
@@ -2529,10 +2523,10 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B139" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C139">
         <v>0</v>
@@ -2543,10 +2537,10 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B140" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C140">
         <v>0</v>
@@ -2557,13 +2551,13 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B141" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C141">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D141" t="b">
         <v>0</v>
@@ -2571,10 +2565,10 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B142" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C142">
         <v>570.46</v>
@@ -2585,10 +2579,10 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B143" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C143">
         <v>0</v>
@@ -2599,10 +2593,10 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B144" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C144">
         <v>0</v>
@@ -2613,13 +2607,13 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B145" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C145">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D145" t="b">
         <v>0</v>
@@ -2627,10 +2621,10 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B146" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C146">
         <v>570.46</v>
@@ -2641,10 +2635,10 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B147" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C147">
         <v>0</v>
@@ -2655,10 +2649,10 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B148" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C148">
         <v>0</v>
@@ -2669,13 +2663,13 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B149" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C149">
-        <v>2103.61</v>
+        <v>2076.4499999999998</v>
       </c>
       <c r="D149" t="b">
         <v>0</v>
@@ -2683,10 +2677,10 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B150" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C150">
         <v>1261.24</v>
@@ -2697,10 +2691,10 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B151" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C151">
         <v>0</v>
@@ -2711,10 +2705,10 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B152" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C152">
         <v>0</v>
@@ -2725,13 +2719,13 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B153" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C153">
-        <v>4539.05</v>
+        <v>1905</v>
       </c>
       <c r="D153" t="b">
         <v>0</v>
@@ -2739,10 +2733,10 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B154" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C154">
         <v>1261.24</v>
@@ -2753,10 +2747,10 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B155" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C155">
         <v>0</v>
@@ -2767,10 +2761,10 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B156" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C156">
         <v>0</v>
@@ -2781,13 +2775,13 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B157" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C157">
-        <v>2691.71</v>
+        <v>1943.11</v>
       </c>
       <c r="D157" t="b">
         <v>0</v>
@@ -2795,10 +2789,10 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B158" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C158">
         <v>2191.36</v>
@@ -2809,10 +2803,10 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B159" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C159">
         <v>0</v>
@@ -2823,13 +2817,13 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B160" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C160">
-        <v>0</v>
+        <v>1159</v>
       </c>
       <c r="D160" t="b">
         <v>0</v>
@@ -2837,13 +2831,13 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B161" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C161">
-        <v>4056.65</v>
+        <v>3525.06</v>
       </c>
       <c r="D161" t="b">
         <v>0</v>
@@ -2851,10 +2845,10 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B162" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C162">
         <v>2191.36</v>
@@ -2865,10 +2859,10 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B163" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C163">
         <v>0</v>
@@ -2879,10 +2873,10 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B164" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C164">
         <v>0</v>
@@ -2893,13 +2887,13 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B165" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C165">
-        <v>3187.53</v>
+        <v>4073.75</v>
       </c>
       <c r="D165" t="b">
         <v>0</v>
@@ -2907,10 +2901,10 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B166" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C166">
         <v>1261.24</v>
@@ -2921,10 +2915,10 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B167" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C167">
         <v>0</v>
@@ -2935,10 +2929,10 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B168" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C168">
         <v>0</v>
@@ -2949,13 +2943,13 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B169" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C169">
-        <v>1904.99</v>
+        <v>1905</v>
       </c>
       <c r="D169" t="b">
         <v>0</v>
@@ -2963,10 +2957,10 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B170" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C170">
         <v>1261.24</v>
@@ -2977,10 +2971,10 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B171" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C171">
         <v>0</v>
@@ -2991,10 +2985,10 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B172" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C172">
         <v>0</v>
@@ -3005,13 +2999,13 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B173" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C173">
-        <v>1904.99</v>
+        <v>1924.05</v>
       </c>
       <c r="D173" t="b">
         <v>0</v>
@@ -3019,10 +3013,10 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B174" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C174">
         <v>1261.24</v>
@@ -3033,10 +3027,10 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B175" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C175">
         <v>0</v>
@@ -3047,10 +3041,10 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B176" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C176">
         <v>0</v>
@@ -3061,13 +3055,13 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B177" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C177">
-        <v>2199.65</v>
+        <v>1905</v>
       </c>
       <c r="D177" t="b">
         <v>0</v>
@@ -3075,10 +3069,10 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B178" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C178">
         <v>2191.36</v>
@@ -3089,10 +3083,10 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B179" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C179">
         <v>0</v>
@@ -3103,10 +3097,10 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B180" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C180">
         <v>0</v>
@@ -3117,10 +3111,10 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B181" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C181">
         <v>1905</v>
@@ -3131,10 +3125,10 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B182" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C182">
         <v>2191.36</v>
@@ -3145,10 +3139,10 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B183" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C183">
         <v>0</v>
@@ -3159,10 +3153,10 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B184" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C184">
         <v>0</v>
@@ -3173,13 +3167,13 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B185" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C185">
-        <v>3711.95</v>
+        <v>3599.86</v>
       </c>
       <c r="D185" t="b">
         <v>0</v>
@@ -3187,10 +3181,10 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B186" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C186">
         <v>2191.36</v>
@@ -3201,10 +3195,10 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B187" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C187">
         <v>0</v>
@@ -3215,10 +3209,10 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B188" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C188">
         <v>0</v>
@@ -3229,13 +3223,13 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B189" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C189">
-        <v>1904.99</v>
+        <v>1943.1</v>
       </c>
       <c r="D189" t="b">
         <v>0</v>
@@ -3243,10 +3237,10 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B190" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C190">
         <v>2191.36</v>
@@ -3257,10 +3251,10 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B191" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C191">
         <v>0</v>
@@ -3271,10 +3265,10 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B192" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C192">
         <v>0</v>
@@ -3285,13 +3279,13 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B193" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C193">
-        <v>1981.18</v>
+        <v>1924.05</v>
       </c>
       <c r="D193" t="b">
         <v>0</v>
@@ -3299,10 +3293,10 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B194" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C194">
         <v>2191.36</v>
@@ -3313,10 +3307,10 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B195" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C195">
         <v>0</v>
@@ -3327,10 +3321,10 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B196" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C196">
         <v>0</v>
@@ -3341,13 +3335,13 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B197" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C197">
-        <v>1904.98</v>
+        <v>1924.05</v>
       </c>
       <c r="D197" t="b">
         <v>0</v>
@@ -3355,10 +3349,10 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B198" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C198">
         <v>1261.24</v>
@@ -3369,10 +3363,10 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B199" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C199">
         <v>0</v>
@@ -3383,10 +3377,10 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B200" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C200">
         <v>0</v>
@@ -3397,13 +3391,13 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B201" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C201">
-        <v>2200.5700000000002</v>
+        <v>2324.1</v>
       </c>
       <c r="D201" t="b">
         <v>0</v>
@@ -3411,10 +3405,10 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B202" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C202">
         <v>1707.7</v>
@@ -3425,10 +3419,10 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B203" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C203">
         <v>0</v>
@@ -3439,13 +3433,13 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B204" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C204">
-        <v>3964</v>
+        <v>1409</v>
       </c>
       <c r="D204" t="b">
         <v>0</v>
@@ -3453,13 +3447,13 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B205" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C205">
-        <v>1904.98</v>
+        <v>3053.4</v>
       </c>
       <c r="D205" t="b">
         <v>0</v>
@@ -3467,10 +3461,10 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B206" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C206">
         <v>1261.24</v>
@@ -3481,10 +3475,10 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B207" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C207">
         <v>0</v>
@@ -3495,10 +3489,10 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B208" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C208">
         <v>0</v>
@@ -3509,10 +3503,10 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B209" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C209">
         <v>1905</v>
@@ -3523,10 +3517,10 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B210" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C210">
         <v>1261.24</v>
@@ -3537,10 +3531,10 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B211" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C211">
         <v>0</v>
@@ -3551,10 +3545,10 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B212" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C212">
         <v>0</v>
@@ -3565,10 +3559,10 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B213" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C213">
         <v>1905</v>
@@ -3579,10 +3573,10 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B214" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C214">
         <v>1261.24</v>
@@ -3593,10 +3587,10 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B215" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C215">
         <v>0</v>
@@ -3607,10 +3601,10 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B216" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C216">
         <v>0</v>
@@ -3621,13 +3615,13 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B217" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C217">
-        <v>2290.85</v>
+        <v>2321.31</v>
       </c>
       <c r="D217" t="b">
         <v>0</v>
@@ -3635,10 +3629,10 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B218" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C218">
         <v>1261.24</v>
@@ -3649,10 +3643,10 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B219" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C219">
         <v>0</v>
@@ -3663,10 +3657,10 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B220" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C220">
         <v>0</v>
@@ -3677,13 +3671,13 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B221" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C221">
-        <v>1904.97</v>
+        <v>1924.05</v>
       </c>
       <c r="D221" t="b">
         <v>0</v>
@@ -3691,10 +3685,10 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B222" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C222">
         <v>1261.24</v>
@@ -3705,10 +3699,10 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B223" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C223">
         <v>0</v>
@@ -3719,10 +3713,10 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B224" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C224">
         <v>0</v>
@@ -3733,13 +3727,13 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B225" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C225">
-        <v>2114.5100000000002</v>
+        <v>2019.3</v>
       </c>
       <c r="D225" t="b">
         <v>0</v>
@@ -3747,10 +3741,10 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B226" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C226">
         <v>1261.24</v>
@@ -3761,10 +3755,10 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B227" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C227">
         <v>0</v>
@@ -3775,10 +3769,10 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B228" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C228">
         <v>0</v>
@@ -3789,13 +3783,13 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B229" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C229">
-        <v>1904.99</v>
+        <v>1943.1</v>
       </c>
       <c r="D229" t="b">
         <v>0</v>
@@ -3803,10 +3797,10 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B230" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C230">
         <v>1261.24</v>
@@ -3817,10 +3811,10 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B231" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C231">
         <v>0</v>
@@ -3831,10 +3825,10 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B232" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C232">
         <v>0</v>
@@ -3845,13 +3839,13 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B233" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C233">
-        <v>2038.32</v>
+        <v>1962.15</v>
       </c>
       <c r="D233" t="b">
         <v>0</v>
@@ -3859,10 +3853,10 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B234" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C234">
         <v>1261.24</v>
@@ -3873,10 +3867,10 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B235" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C235">
         <v>0</v>
@@ -3887,10 +3881,10 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B236" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C236">
         <v>0</v>
@@ -3901,13 +3895,13 @@
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B237" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C237">
-        <v>1924.04</v>
+        <v>1924.05</v>
       </c>
       <c r="D237" t="b">
         <v>0</v>
@@ -3915,10 +3909,10 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B238" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C238">
         <v>1261.24</v>
@@ -3929,10 +3923,10 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B239" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C239">
         <v>0</v>
@@ -3943,10 +3937,10 @@
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B240" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C240">
         <v>0</v>
@@ -3957,13 +3951,13 @@
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B241" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C241">
-        <v>2381.2399999999998</v>
+        <v>2000.25</v>
       </c>
       <c r="D241" t="b">
         <v>0</v>
@@ -3971,10 +3965,10 @@
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B242" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C242">
         <v>1261.24</v>
@@ -3985,10 +3979,10 @@
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B243" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C243">
         <v>0</v>
@@ -3999,10 +3993,10 @@
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B244" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C244">
         <v>0</v>
@@ -4013,13 +4007,13 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B245" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C245">
-        <v>1904.99</v>
+        <v>1905</v>
       </c>
       <c r="D245" t="b">
         <v>0</v>
@@ -4027,10 +4021,10 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B246" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C246">
         <v>1261.24</v>
@@ -4041,10 +4035,10 @@
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B247" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C247">
         <v>0</v>
@@ -4055,10 +4049,10 @@
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B248" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C248">
         <v>0</v>
@@ -4069,13 +4063,13 @@
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B249" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C249">
-        <v>1962.12</v>
+        <v>2006.63</v>
       </c>
       <c r="D249" t="b">
         <v>0</v>
@@ -4083,10 +4077,10 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B250" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C250">
         <v>1261.24</v>
@@ -4097,10 +4091,10 @@
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B251" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C251">
         <v>0</v>
@@ -4111,10 +4105,10 @@
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B252" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C252">
         <v>0</v>
@@ -4125,13 +4119,13 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B253" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C253">
-        <v>1924</v>
+        <v>2785.5</v>
       </c>
       <c r="D253" t="b">
         <v>0</v>
@@ -4139,10 +4133,10 @@
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B254" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C254">
         <v>2191.36</v>
@@ -4153,10 +4147,10 @@
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B255" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C255">
         <v>0</v>
@@ -4167,10 +4161,10 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B256" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C256">
         <v>0</v>
@@ -4181,13 +4175,13 @@
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B257" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C257">
-        <v>4057.62</v>
+        <v>3790.97</v>
       </c>
       <c r="D257" t="b">
         <v>0</v>
@@ -4195,10 +4189,10 @@
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B258" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C258">
         <v>2191.36</v>
@@ -4209,10 +4203,10 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B259" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C259">
         <v>0</v>
@@ -4223,13 +4217,13 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B260" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C260">
-        <v>5809</v>
+        <v>7639</v>
       </c>
       <c r="D260" t="b">
         <v>0</v>
@@ -4237,13 +4231,13 @@
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B261" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C261">
-        <v>1924.04</v>
+        <v>1905</v>
       </c>
       <c r="D261" t="b">
         <v>0</v>
@@ -4251,10 +4245,10 @@
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B262" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C262">
         <v>1261.24</v>
@@ -4265,10 +4259,10 @@
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B263" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C263">
         <v>0</v>
@@ -4279,10 +4273,10 @@
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B264" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C264">
         <v>0</v>
@@ -4293,13 +4287,13 @@
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B265" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C265">
-        <v>2240.2800000000002</v>
+        <v>3097.76</v>
       </c>
       <c r="D265" t="b">
         <v>0</v>
@@ -4307,13 +4301,13 @@
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B266" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C266">
-        <v>1979.29</v>
+        <v>2191.36</v>
       </c>
       <c r="D266" t="b">
         <v>0</v>
@@ -4321,10 +4315,10 @@
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B267" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C267">
         <v>0</v>
@@ -4335,10 +4329,10 @@
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B268" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C268">
         <v>0</v>
@@ -4349,13 +4343,13 @@
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B269" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C269">
-        <v>10569.49</v>
+        <v>1943.1</v>
       </c>
       <c r="D269" t="b">
         <v>0</v>
@@ -4363,13 +4357,13 @@
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B270" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C270">
-        <v>2191.36</v>
+        <v>1261.24</v>
       </c>
       <c r="D270" t="b">
         <v>0</v>
@@ -4377,10 +4371,10 @@
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B271" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C271">
         <v>0</v>
@@ -4391,10 +4385,10 @@
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B272" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C272">
         <v>0</v>
@@ -4405,13 +4399,13 @@
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B273" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C273">
-        <v>2038.34</v>
+        <v>1905</v>
       </c>
       <c r="D273" t="b">
         <v>0</v>
@@ -4419,13 +4413,13 @@
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B274" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C274">
-        <v>1261.24</v>
+        <v>2191.36</v>
       </c>
       <c r="D274" t="b">
         <v>0</v>
@@ -4433,10 +4427,10 @@
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B275" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C275">
         <v>0</v>
@@ -4447,10 +4441,10 @@
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B276" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C276">
         <v>0</v>
@@ -4461,13 +4455,13 @@
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B277" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C277">
-        <v>2038.32</v>
+        <v>2133.6</v>
       </c>
       <c r="D277" t="b">
         <v>0</v>
@@ -4475,13 +4469,13 @@
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B278" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C278">
-        <v>2191.36</v>
+        <v>1261.24</v>
       </c>
       <c r="D278" t="b">
         <v>0</v>
@@ -4489,10 +4483,10 @@
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B279" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C279">
         <v>0</v>
@@ -4503,10 +4497,10 @@
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B280" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C280">
         <v>0</v>
@@ -4517,13 +4511,13 @@
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B281" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C281">
-        <v>2057.38</v>
+        <v>1943.1</v>
       </c>
       <c r="D281" t="b">
         <v>0</v>
@@ -4531,10 +4525,10 @@
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B282" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C282">
         <v>1261.24</v>
@@ -4545,10 +4539,10 @@
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B283" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C283">
         <v>0</v>
@@ -4559,10 +4553,10 @@
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B284" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C284">
         <v>0</v>
@@ -4573,10 +4567,10 @@
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B285" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C285">
         <v>1905</v>
@@ -4587,13 +4581,13 @@
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B286" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C286">
-        <v>1261.24</v>
+        <v>2191.36</v>
       </c>
       <c r="D286" t="b">
         <v>0</v>
@@ -4601,10 +4595,10 @@
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B287" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C287">
         <v>0</v>
@@ -4615,10 +4609,10 @@
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B288" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C288">
         <v>0</v>
@@ -4629,13 +4623,13 @@
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B289" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C289">
-        <v>1904.98</v>
+        <v>1924.05</v>
       </c>
       <c r="D289" t="b">
         <v>0</v>
@@ -4643,13 +4637,13 @@
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B290" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C290">
-        <v>2191.36</v>
+        <v>1261.24</v>
       </c>
       <c r="D290" t="b">
         <v>0</v>
@@ -4657,10 +4651,10 @@
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B291" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C291">
         <v>0</v>
@@ -4671,10 +4665,10 @@
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B292" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C292">
         <v>0</v>
@@ -4685,13 +4679,13 @@
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B293" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C293">
-        <v>1943.07</v>
+        <v>1905</v>
       </c>
       <c r="D293" t="b">
         <v>0</v>
@@ -4699,10 +4693,10 @@
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B294" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C294">
         <v>1261.24</v>
@@ -4713,10 +4707,10 @@
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B295" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C295">
         <v>0</v>
@@ -4727,10 +4721,10 @@
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B296" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C296">
         <v>0</v>
@@ -4741,13 +4735,13 @@
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B297" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C297">
-        <v>1924.04</v>
+        <v>3453.41</v>
       </c>
       <c r="D297" t="b">
         <v>0</v>
@@ -4755,10 +4749,10 @@
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B298" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C298">
         <v>1261.24</v>
@@ -4769,13 +4763,13 @@
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B299" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C299">
-        <v>0</v>
+        <v>1387</v>
       </c>
       <c r="D299" t="b">
         <v>0</v>
@@ -4783,13 +4777,13 @@
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B300" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C300">
-        <v>0</v>
+        <v>8163</v>
       </c>
       <c r="D300" t="b">
         <v>0</v>
@@ -4797,13 +4791,13 @@
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B301" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C301">
-        <v>3415.25</v>
+        <v>2343.15</v>
       </c>
       <c r="D301" t="b">
         <v>0</v>
@@ -4811,10 +4805,10 @@
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B302" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C302">
         <v>1261.24</v>
@@ -4825,10 +4819,10 @@
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B303" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C303">
         <v>0</v>
@@ -4839,13 +4833,13 @@
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B304" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C304">
-        <v>19438</v>
+        <v>0</v>
       </c>
       <c r="D304" t="b">
         <v>0</v>
@@ -4853,13 +4847,13 @@
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B305" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C305">
-        <v>2228.81</v>
+        <v>1981.2</v>
       </c>
       <c r="D305" t="b">
         <v>0</v>
@@ -4867,10 +4861,10 @@
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B306" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C306">
         <v>1261.24</v>
@@ -4881,10 +4875,10 @@
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B307" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C307">
         <v>0</v>
@@ -4895,71 +4889,15 @@
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B308" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C308">
-        <v>1093</v>
+        <v>0</v>
       </c>
       <c r="D308" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A309" t="s">
-        <v>81</v>
-      </c>
-      <c r="B309" t="s">
-        <v>1</v>
-      </c>
-      <c r="C309">
-        <v>1962.13</v>
-      </c>
-      <c r="D309" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A310" t="s">
-        <v>81</v>
-      </c>
-      <c r="B310" t="s">
-        <v>2</v>
-      </c>
-      <c r="C310">
-        <v>1261.24</v>
-      </c>
-      <c r="D310" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A311" t="s">
-        <v>81</v>
-      </c>
-      <c r="B311" t="s">
-        <v>3</v>
-      </c>
-      <c r="C311">
-        <v>0</v>
-      </c>
-      <c r="D311" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A312" t="s">
-        <v>81</v>
-      </c>
-      <c r="B312" t="s">
-        <v>4</v>
-      </c>
-      <c r="C312">
-        <v>0</v>
-      </c>
-      <c r="D312" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>